<commit_message>
Update get unit price foreach class lecturer taught
</commit_message>
<xml_diff>
--- a/TeachingAssignmentManagement/Uploads/CNTT ThoiKhoaBieu_HK222_Nganh7480201-DB.xlsx
+++ b/TeachingAssignmentManagement/Uploads/CNTT ThoiKhoaBieu_HK222_Nganh7480201-DB.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:si>
     <x:t>MaGocLHP</x:t>
   </x:si>
@@ -106,21 +106,186 @@
     <x:t>Ghi chú 2</x:t>
   </x:si>
   <x:si>
+    <x:t>222_72ITBS20203_01</x:t>
+  </x:si>
+  <x:si>
+    <x:t>72ITBS20203-222-7480201-DB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cơ sở lập trình</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Lý thuyết</x:t>
+  </x:si>
+  <x:si>
+    <x:t>72K28CNTT01</x:t>
+  </x:si>
+  <x:si>
+    <x:t>60</x:t>
+  </x:si>
+  <x:si>
+    <x:t>30</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Thứ Tư</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1 - 3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CS3.G.08.29</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2001100112</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Nguyễn Văn Trung</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PMT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Được chấp nhận</x:t>
+  </x:si>
+  <x:si>
+    <x:t>26,27,28,29,30,31,32,33,34,35</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>26</x:t>
+  </x:si>
+  <x:si>
+    <x:t>35</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Thứ Bảy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>222_72ITMA20403_01</x:t>
+  </x:si>
+  <x:si>
+    <x:t>72ITMA20403-222-7480201-DB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Toán rời rạc</x:t>
+  </x:si>
+  <x:si>
+    <x:t>72K27CNTT01</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Thứ Năm</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4 - 6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CS3.G.10.02</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2001101105</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Phan Hồ Viết Trường</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PLT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>40</x:t>
+  </x:si>
+  <x:si>
+    <x:t>17,18,19,23,24,25,26,27,28,29</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>17</x:t>
+  </x:si>
+  <x:si>
+    <x:t>29</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CS3.G.10.07</x:t>
+  </x:si>
+  <x:si>
+    <x:t>222_72ITSE30303_01</x:t>
+  </x:si>
+  <x:si>
+    <x:t>72ITSE30303-222-7480201-DB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cấu trúc dữ liệu và giải thuật</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Thứ Ba</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2001102317</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Huỳnh Anh Dũng</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Thứ Sáu</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2001101100</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Nguyễn Minh Tân</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>222_72ITSE41003_01</x:t>
+  </x:si>
+  <x:si>
+    <x:t>72ITSE41003-222-7480201-DB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Nhập môn công nghệ phần mềm</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CS3.G.08.11</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2001100008</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Bùi Minh Phụng</x:t>
+  </x:si>
+  <x:si>
     <x:t>222_72HBDC10073_01</x:t>
   </x:si>
   <x:si>
-    <x:t>72HBDC10073</x:t>
+    <x:t>72HBDC10073-222-7480201-DB</x:t>
   </x:si>
   <x:si>
     <x:t>Trở thành công dân số</x:t>
   </x:si>
   <x:si>
-    <x:t>3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Lý thuyết</x:t>
-  </x:si>
-  <x:si>
     <x:t>72K27CNTT01, 72K27KDTM01, 72K27KETO01, 72K27KTRU01, 72K27MARK01, 72K27NGNA01, 72K27QHCC01, 72K27QTKD01, 72K27TKDH01, 72K27TKDH02</x:t>
   </x:si>
   <x:si>
@@ -130,36 +295,21 @@
     <x:t>36</x:t>
   </x:si>
   <x:si>
-    <x:t>Thứ Ba</x:t>
-  </x:si>
-  <x:si>
-    <x:t>7</x:t>
-  </x:si>
-  <x:si>
     <x:t>7 - 9</x:t>
   </x:si>
   <x:si>
     <x:t>CS3.G.10.06</x:t>
   </x:si>
   <x:si>
-    <x:t>PLT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>40</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Được chấp nhận</x:t>
+    <x:t>2001100724</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Huỳnh Thanh Tuấn</x:t>
   </x:si>
   <x:si>
     <x:t>17,18,19,23,24,25,26,27,28,29,30,31</x:t>
   </x:si>
   <x:si>
-    <x:t>17</x:t>
-  </x:si>
-  <x:si>
     <x:t>31</x:t>
   </x:si>
   <x:si>
@@ -178,148 +328,16 @@
     <x:t>222_72HBDC10073_03</x:t>
   </x:si>
   <x:si>
-    <x:t>Thứ Năm</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5</x:t>
+    <x:t>2001100428</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Hà Đồng Hưng</x:t>
   </x:si>
   <x:si>
     <x:t>222_72HBDC10073_04</x:t>
   </x:si>
   <x:si>
     <x:t>CS3.G.10.01</x:t>
-  </x:si>
-  <x:si>
-    <x:t>222_72ITBS20203_01</x:t>
-  </x:si>
-  <x:si>
-    <x:t>72ITBS20203</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Cơ sở lập trình</x:t>
-  </x:si>
-  <x:si>
-    <x:t>72K28CNTT01</x:t>
-  </x:si>
-  <x:si>
-    <x:t>60</x:t>
-  </x:si>
-  <x:si>
-    <x:t>30</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Thứ Tư</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1 - 3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CS3.G.08.29</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2001100112</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Nguyễn Văn Trung</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PMT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>26,27,28,29,30,31,32,33,34,35</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>26</x:t>
-  </x:si>
-  <x:si>
-    <x:t>35</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Thứ Bảy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>222_72ITMA20403_01</x:t>
-  </x:si>
-  <x:si>
-    <x:t>72ITMA20403</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Toán rời rạc</x:t>
-  </x:si>
-  <x:si>
-    <x:t>72K27CNTT01</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4 - 6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CS3.G.10.02</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2001101105</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Phan Hồ Viết Trường</x:t>
-  </x:si>
-  <x:si>
-    <x:t>17,18,19,23,24,25,26,27,28,29</x:t>
-  </x:si>
-  <x:si>
-    <x:t>29</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CS3.G.10.07</x:t>
-  </x:si>
-  <x:si>
-    <x:t>222_72ITSE30303_01</x:t>
-  </x:si>
-  <x:si>
-    <x:t>72ITSE30303</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Cấu trúc dữ liệu và giải thuật</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2001101100</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Nguyễn Minh Tân</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Thứ Sáu</x:t>
-  </x:si>
-  <x:si>
-    <x:t>6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>222_72ITSE41003_01</x:t>
-  </x:si>
-  <x:si>
-    <x:t>72ITSE41003</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Nhập môn công nghệ phần mềm</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CS3.G.08.11</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2001100008</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Bùi Minh Phụng</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -877,54 +895,55 @@
       <x:c r="O2" s="0" t="s">
         <x:v>41</x:v>
       </x:c>
-      <x:c r="P2" s="2" t="s"/>
-      <x:c r="Q2" s="2" t="s"/>
+      <x:c r="P2" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="Q2" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
       <x:c r="R2" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="S2" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="T2" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="U2" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="V2" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="W2" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="X2" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="Y2" s="0" t="s">
         <x:v>39</x:v>
       </x:c>
       <x:c r="Z2" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="AA2" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="AB2" s="0" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="AC2" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>52</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:30">
       <x:c r="A3" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
         <x:v>31</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
         <x:v>32</x:v>
@@ -945,71 +964,72 @@
         <x:v>37</x:v>
       </x:c>
       <x:c r="K3" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="L3" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="M3" s="0" t="s">
         <x:v>33</x:v>
       </x:c>
       <x:c r="N3" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="O3" s="0" t="s">
         <x:v>41</x:v>
       </x:c>
-      <x:c r="P3" s="2" t="s"/>
-      <x:c r="Q3" s="2" t="s"/>
+      <x:c r="P3" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="Q3" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
       <x:c r="R3" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="S3" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="T3" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="U3" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="V3" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="W3" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="X3" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="Y3" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="Z3" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="AA3" s="0" t="s">
         <x:v>51</x:v>
       </x:c>
-      <x:c r="Z3" s="0" t="s">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c r="AA3" s="0" t="s">
-        <x:v>47</x:v>
-      </x:c>
       <x:c r="AB3" s="0" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="AC3" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>52</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:30">
       <x:c r="A4" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="E4" s="0" t="s">
         <x:v>33</x:v>
@@ -1018,7 +1038,7 @@
         <x:v>34</x:v>
       </x:c>
       <x:c r="G4" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="H4" s="0" t="s">
         <x:v>36</x:v>
@@ -1027,71 +1047,72 @@
         <x:v>37</x:v>
       </x:c>
       <x:c r="K4" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="L4" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="M4" s="0" t="s">
         <x:v>33</x:v>
       </x:c>
       <x:c r="N4" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="O4" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="P4" s="2" t="s"/>
-      <x:c r="Q4" s="2" t="s"/>
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="P4" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="Q4" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
       <x:c r="R4" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="S4" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="T4" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="U4" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="V4" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="W4" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="X4" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="Y4" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="Z4" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="AA4" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="AB4" s="0" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="AC4" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>69</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:30">
       <x:c r="A5" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
         <x:v>56</x:v>
       </x:c>
-      <x:c r="B5" s="0" t="s">
-        <x:v>31</x:v>
-      </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="E5" s="0" t="s">
         <x:v>33</x:v>
@@ -1100,7 +1121,7 @@
         <x:v>34</x:v>
       </x:c>
       <x:c r="G5" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="H5" s="0" t="s">
         <x:v>36</x:v>
@@ -1109,71 +1130,72 @@
         <x:v>37</x:v>
       </x:c>
       <x:c r="K5" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="L5" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="M5" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="N5" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="O5" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="P5" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="Q5" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="R5" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="S5" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="T5" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="U5" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="V5" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="W5" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="X5" s="0" t="s">
         <x:v>54</x:v>
       </x:c>
-      <x:c r="L5" s="0" t="s">
-        <x:v>51</x:v>
-      </x:c>
-      <x:c r="M5" s="0" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="N5" s="0" t="s">
-        <x:v>52</x:v>
-      </x:c>
-      <x:c r="O5" s="0" t="s">
-        <x:v>57</x:v>
-      </x:c>
-      <x:c r="P5" s="2" t="s"/>
-      <x:c r="Q5" s="2" t="s"/>
-      <x:c r="R5" s="0" t="s">
-        <x:v>42</x:v>
-      </x:c>
-      <x:c r="S5" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="T5" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="U5" s="0" t="s">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c r="V5" s="0" t="s">
-        <x:v>45</x:v>
-      </x:c>
-      <x:c r="W5" s="0" t="s">
-        <x:v>46</x:v>
-      </x:c>
-      <x:c r="X5" s="0" t="s">
-        <x:v>55</x:v>
-      </x:c>
       <x:c r="Y5" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="Z5" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="AA5" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="AB5" s="0" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="AC5" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>69</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:30">
       <x:c r="A6" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="E6" s="0" t="s">
         <x:v>33</x:v>
@@ -1182,81 +1204,81 @@
         <x:v>34</x:v>
       </x:c>
       <x:c r="G6" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="H6" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="I6" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="K6" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="L6" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="M6" s="0" t="s">
         <x:v>33</x:v>
       </x:c>
       <x:c r="N6" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="O6" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="P6" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="Q6" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="R6" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="S6" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="T6" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="U6" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="V6" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="W6" s="0" t="s">
         <x:v>66</x:v>
       </x:c>
-      <x:c r="O6" s="0" t="s">
-        <x:v>67</x:v>
-      </x:c>
-      <x:c r="P6" s="0" t="s">
+      <x:c r="X6" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="Y6" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="Z6" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="AA6" s="0" t="s">
         <x:v>68</x:v>
       </x:c>
-      <x:c r="Q6" s="0" t="s">
+      <x:c r="AB6" s="0" t="s">
         <x:v>69</x:v>
-      </x:c>
-      <x:c r="R6" s="0" t="s">
-        <x:v>70</x:v>
-      </x:c>
-      <x:c r="S6" s="0" t="s">
-        <x:v>71</x:v>
-      </x:c>
-      <x:c r="T6" s="0" t="s">
-        <x:v>63</x:v>
-      </x:c>
-      <x:c r="U6" s="0" t="s">
-        <x:v>72</x:v>
-      </x:c>
-      <x:c r="V6" s="0" t="s">
-        <x:v>45</x:v>
-      </x:c>
-      <x:c r="W6" s="0" t="s">
-        <x:v>73</x:v>
-      </x:c>
-      <x:c r="X6" s="0" t="s">
-        <x:v>74</x:v>
-      </x:c>
-      <x:c r="Y6" s="0" t="s">
-        <x:v>65</x:v>
-      </x:c>
-      <x:c r="Z6" s="0" t="s">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c r="AA6" s="0" t="s">
-        <x:v>75</x:v>
-      </x:c>
-      <x:c r="AB6" s="0" t="s">
-        <x:v>76</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:30">
       <x:c r="A7" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="E7" s="0" t="s">
         <x:v>33</x:v>
@@ -1265,81 +1287,81 @@
         <x:v>34</x:v>
       </x:c>
       <x:c r="G7" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="H7" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="I7" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="K7" s="0" t="s">
         <x:v>77</x:v>
       </x:c>
       <x:c r="L7" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="M7" s="0" t="s">
         <x:v>33</x:v>
       </x:c>
       <x:c r="N7" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="O7" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="P7" s="0" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="Q7" s="0" t="s">
+        <x:v>79</x:v>
+      </x:c>
+      <x:c r="R7" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="S7" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="T7" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="U7" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="V7" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="W7" s="0" t="s">
         <x:v>66</x:v>
       </x:c>
-      <x:c r="O7" s="0" t="s">
-        <x:v>67</x:v>
-      </x:c>
-      <x:c r="P7" s="0" t="s">
+      <x:c r="X7" s="0" t="s">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="Y7" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="Z7" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="AA7" s="0" t="s">
         <x:v>68</x:v>
       </x:c>
-      <x:c r="Q7" s="0" t="s">
+      <x:c r="AB7" s="0" t="s">
         <x:v>69</x:v>
-      </x:c>
-      <x:c r="R7" s="0" t="s">
-        <x:v>70</x:v>
-      </x:c>
-      <x:c r="S7" s="0" t="s">
-        <x:v>71</x:v>
-      </x:c>
-      <x:c r="T7" s="0" t="s">
-        <x:v>63</x:v>
-      </x:c>
-      <x:c r="U7" s="0" t="s">
-        <x:v>72</x:v>
-      </x:c>
-      <x:c r="V7" s="0" t="s">
-        <x:v>45</x:v>
-      </x:c>
-      <x:c r="W7" s="0" t="s">
-        <x:v>73</x:v>
-      </x:c>
-      <x:c r="X7" s="0" t="s">
-        <x:v>39</x:v>
-      </x:c>
-      <x:c r="Y7" s="0" t="s">
-        <x:v>65</x:v>
-      </x:c>
-      <x:c r="Z7" s="0" t="s">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c r="AA7" s="0" t="s">
-        <x:v>75</x:v>
-      </x:c>
-      <x:c r="AB7" s="0" t="s">
-        <x:v>76</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:30">
       <x:c r="A8" s="0" t="s">
-        <x:v>78</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>79</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>78</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>80</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="E8" s="0" t="s">
         <x:v>33</x:v>
@@ -1348,81 +1370,81 @@
         <x:v>34</x:v>
       </x:c>
       <x:c r="G8" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="H8" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="I8" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="K8" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="L8" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="M8" s="0" t="s">
         <x:v>33</x:v>
       </x:c>
       <x:c r="N8" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="O8" s="0" t="s">
-        <x:v>83</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="P8" s="0" t="s">
-        <x:v>84</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="Q8" s="0" t="s">
-        <x:v>85</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="R8" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="S8" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="T8" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="U8" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="V8" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="W8" s="0" t="s">
-        <x:v>86</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="X8" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="Y8" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="Z8" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="AA8" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="AB8" s="0" t="s">
-        <x:v>87</x:v>
+        <x:v>69</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:30">
       <x:c r="A9" s="0" t="s">
-        <x:v>78</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>79</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>78</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>80</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="E9" s="0" t="s">
         <x:v>33</x:v>
@@ -1431,81 +1453,81 @@
         <x:v>34</x:v>
       </x:c>
       <x:c r="G9" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="H9" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="I9" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="K9" s="0" t="s">
         <x:v>77</x:v>
       </x:c>
       <x:c r="L9" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="M9" s="0" t="s">
         <x:v>33</x:v>
       </x:c>
       <x:c r="N9" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="O9" s="0" t="s">
-        <x:v>88</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="P9" s="0" t="s">
-        <x:v>84</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="Q9" s="0" t="s">
-        <x:v>85</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="R9" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="S9" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="T9" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="U9" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="V9" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="W9" s="0" t="s">
-        <x:v>86</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="X9" s="0" t="s">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="Y9" s="0" t="s">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="Y9" s="0" t="s">
-        <x:v>74</x:v>
-      </x:c>
       <x:c r="Z9" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="AA9" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="AB9" s="0" t="s">
-        <x:v>87</x:v>
+        <x:v>69</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:30">
       <x:c r="A10" s="0" t="s">
+        <x:v>87</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
+        <x:v>87</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
         <x:v>89</x:v>
-      </x:c>
-      <x:c r="B10" s="0" t="s">
-        <x:v>90</x:v>
-      </x:c>
-      <x:c r="C10" s="0" t="s">
-        <x:v>89</x:v>
-      </x:c>
-      <x:c r="D10" s="0" t="s">
-        <x:v>91</x:v>
       </x:c>
       <x:c r="E10" s="0" t="s">
         <x:v>33</x:v>
@@ -1514,81 +1536,84 @@
         <x:v>34</x:v>
       </x:c>
       <x:c r="G10" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="H10" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="I10" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="K10" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="L10" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="M10" s="0" t="s">
         <x:v>33</x:v>
       </x:c>
       <x:c r="N10" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="O10" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="P10" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="Q10" s="0" t="s">
-        <x:v>93</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="R10" s="0" t="s">
-        <x:v>70</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="S10" s="0" t="s">
-        <x:v>71</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="T10" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="U10" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="V10" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="W10" s="0" t="s">
-        <x:v>86</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="X10" s="0" t="s">
         <x:v>33</x:v>
       </x:c>
       <x:c r="Y10" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="Z10" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="AA10" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="AB10" s="0" t="s">
-        <x:v>87</x:v>
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="AC10" s="0" t="s">
+        <x:v>99</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:30">
       <x:c r="A11" s="0" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
         <x:v>89</x:v>
-      </x:c>
-      <x:c r="B11" s="0" t="s">
-        <x:v>90</x:v>
-      </x:c>
-      <x:c r="C11" s="0" t="s">
-        <x:v>89</x:v>
-      </x:c>
-      <x:c r="D11" s="0" t="s">
-        <x:v>91</x:v>
       </x:c>
       <x:c r="E11" s="0" t="s">
         <x:v>33</x:v>
@@ -1597,81 +1622,80 @@
         <x:v>34</x:v>
       </x:c>
       <x:c r="G11" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="H11" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="I11" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="K11" s="0" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="L11" s="0" t="s">
+        <x:v>101</x:v>
+      </x:c>
+      <x:c r="M11" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="N11" s="0" t="s">
+        <x:v>102</x:v>
+      </x:c>
+      <x:c r="O11" s="0" t="s">
         <x:v>94</x:v>
       </x:c>
-      <x:c r="L11" s="0" t="s">
-        <x:v>74</x:v>
-      </x:c>
-      <x:c r="M11" s="0" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="N11" s="0" t="s">
-        <x:v>82</x:v>
-      </x:c>
-      <x:c r="O11" s="0" t="s">
-        <x:v>67</x:v>
-      </x:c>
-      <x:c r="P11" s="0" t="s">
-        <x:v>92</x:v>
-      </x:c>
-      <x:c r="Q11" s="0" t="s">
-        <x:v>93</x:v>
-      </x:c>
+      <x:c r="P11" s="2" t="s"/>
+      <x:c r="Q11" s="2" t="s"/>
       <x:c r="R11" s="0" t="s">
-        <x:v>70</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="S11" s="0" t="s">
-        <x:v>71</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="T11" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="U11" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="V11" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="W11" s="0" t="s">
-        <x:v>86</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="X11" s="0" t="s">
-        <x:v>95</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="Y11" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="Z11" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="AA11" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="AB11" s="0" t="s">
-        <x:v>87</x:v>
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="AC11" s="0" t="s">
+        <x:v>99</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:30">
       <x:c r="A12" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>97</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>98</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="E12" s="0" t="s">
         <x:v>33</x:v>
@@ -1680,81 +1704,84 @@
         <x:v>34</x:v>
       </x:c>
       <x:c r="G12" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="H12" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="I12" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="K12" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="L12" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="M12" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="N12" s="0" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="O12" s="0" t="s">
+        <x:v>94</x:v>
+      </x:c>
+      <x:c r="P12" s="0" t="s">
+        <x:v>104</x:v>
+      </x:c>
+      <x:c r="Q12" s="0" t="s">
+        <x:v>105</x:v>
+      </x:c>
+      <x:c r="R12" s="0" t="s">
         <x:v>64</x:v>
       </x:c>
-      <x:c r="L12" s="0" t="s">
-        <x:v>74</x:v>
-      </x:c>
-      <x:c r="M12" s="0" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="N12" s="0" t="s">
-        <x:v>82</x:v>
-      </x:c>
-      <x:c r="O12" s="0" t="s">
+      <x:c r="S12" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="T12" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="U12" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="V12" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="W12" s="0" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="X12" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="Y12" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="Z12" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="AA12" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="AB12" s="0" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="AC12" s="0" t="s">
         <x:v>99</x:v>
-      </x:c>
-      <x:c r="P12" s="0" t="s">
-        <x:v>100</x:v>
-      </x:c>
-      <x:c r="Q12" s="0" t="s">
-        <x:v>101</x:v>
-      </x:c>
-      <x:c r="R12" s="0" t="s">
-        <x:v>70</x:v>
-      </x:c>
-      <x:c r="S12" s="0" t="s">
-        <x:v>71</x:v>
-      </x:c>
-      <x:c r="T12" s="0" t="s">
-        <x:v>63</x:v>
-      </x:c>
-      <x:c r="U12" s="0" t="s">
-        <x:v>72</x:v>
-      </x:c>
-      <x:c r="V12" s="0" t="s">
-        <x:v>45</x:v>
-      </x:c>
-      <x:c r="W12" s="0" t="s">
-        <x:v>86</x:v>
-      </x:c>
-      <x:c r="X12" s="0" t="s">
-        <x:v>74</x:v>
-      </x:c>
-      <x:c r="Y12" s="0" t="s">
-        <x:v>74</x:v>
-      </x:c>
-      <x:c r="Z12" s="0" t="s">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c r="AA12" s="0" t="s">
-        <x:v>47</x:v>
-      </x:c>
-      <x:c r="AB12" s="0" t="s">
-        <x:v>87</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:30">
       <x:c r="A13" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>97</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
-        <x:v>98</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="E13" s="0" t="s">
         <x:v>33</x:v>
@@ -1763,67 +1790,70 @@
         <x:v>34</x:v>
       </x:c>
       <x:c r="G13" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="H13" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="I13" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="K13" s="0" t="s">
-        <x:v>94</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="L13" s="0" t="s">
+        <x:v>101</x:v>
+      </x:c>
+      <x:c r="M13" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="N13" s="0" t="s">
+        <x:v>102</x:v>
+      </x:c>
+      <x:c r="O13" s="0" t="s">
+        <x:v>107</x:v>
+      </x:c>
+      <x:c r="P13" s="0" t="s">
+        <x:v>104</x:v>
+      </x:c>
+      <x:c r="Q13" s="0" t="s">
+        <x:v>105</x:v>
+      </x:c>
+      <x:c r="R13" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="S13" s="0" t="s">
         <x:v>65</x:v>
       </x:c>
-      <x:c r="M13" s="0" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="N13" s="0" t="s">
-        <x:v>66</x:v>
-      </x:c>
-      <x:c r="O13" s="0" t="s">
+      <x:c r="T13" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="U13" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="V13" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="W13" s="0" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="X13" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="Y13" s="0" t="s">
+        <x:v>101</x:v>
+      </x:c>
+      <x:c r="Z13" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="AA13" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="AB13" s="0" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="AC13" s="0" t="s">
         <x:v>99</x:v>
-      </x:c>
-      <x:c r="P13" s="0" t="s">
-        <x:v>100</x:v>
-      </x:c>
-      <x:c r="Q13" s="0" t="s">
-        <x:v>101</x:v>
-      </x:c>
-      <x:c r="R13" s="0" t="s">
-        <x:v>70</x:v>
-      </x:c>
-      <x:c r="S13" s="0" t="s">
-        <x:v>71</x:v>
-      </x:c>
-      <x:c r="T13" s="0" t="s">
-        <x:v>63</x:v>
-      </x:c>
-      <x:c r="U13" s="0" t="s">
-        <x:v>72</x:v>
-      </x:c>
-      <x:c r="V13" s="0" t="s">
-        <x:v>45</x:v>
-      </x:c>
-      <x:c r="W13" s="0" t="s">
-        <x:v>86</x:v>
-      </x:c>
-      <x:c r="X13" s="0" t="s">
-        <x:v>95</x:v>
-      </x:c>
-      <x:c r="Y13" s="0" t="s">
-        <x:v>65</x:v>
-      </x:c>
-      <x:c r="Z13" s="0" t="s">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c r="AA13" s="0" t="s">
-        <x:v>47</x:v>
-      </x:c>
-      <x:c r="AB13" s="0" t="s">
-        <x:v>87</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>